<commit_message>
Finished TST2770 499 589 721 831 993
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/TST589_UsersCanEditAnActionSetsIfTheyHaveRightsToAllActionTypesWithinTheSet.xlsx
+++ b/NformTester/NformTester/Keywordscripts/TST589_UsersCanEditAnActionSetsIfTheyHaveRightsToAllActionTypesWithinTheSet.xlsx
@@ -1210,7 +1210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7476" uniqueCount="854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7798" uniqueCount="877">
   <si>
     <t>FormLogin_to_LiebertR_Nform</t>
   </si>
@@ -3609,10 +3609,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>"Users"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>C</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -3677,27 +3673,7 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>VerifyProperty</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Text</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Equal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Users</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>;T</t>
-  </si>
-  <si>
-    <t>"Users"</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>"All Devices"</t>
@@ -3736,10 +3712,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>;Go to Configure-&gt;Actions.</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3748,10 +3720,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>;Login Nform by Admin user</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>Application</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -3832,11 +3800,115 @@
     <t>Result</t>
   </si>
   <si>
-    <t>;Action</t>
+    <t>"Users"</t>
+  </si>
+  <si>
+    <t>T</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>66</t>
+    <t>"Operator rights test"</t>
+  </si>
+  <si>
+    <t>"Custom group"</t>
+  </si>
+  <si>
+    <t>"Operator rights"</t>
+  </si>
+  <si>
+    <t>;Create custom group  with all actions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"nform"</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>"test-writefile"</t>
+  </si>
+  <si>
+    <t>"nform testing"</t>
+  </si>
+  <si>
+    <t>"abc"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"text"</t>
+  </si>
+  <si>
+    <t>"99"</t>
+  </si>
+  <si>
+    <t>"Unicode"</t>
+  </si>
+  <si>
+    <t>"Unicode (Big-Endian)"</t>
+  </si>
+  <si>
+    <t>"Unicode (UTF-8)"</t>
+  </si>
+  <si>
+    <t>"US-ASCII"</t>
+  </si>
+  <si>
+    <t>"Western European (ISO)"</t>
+  </si>
+  <si>
+    <t>"2"</t>
+  </si>
+  <si>
+    <t>"C:\Nform\result.dat"</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>"edit nform testing"</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>edit nform testing</t>
+  </si>
+  <si>
+    <t>;T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Test"</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"TestDescription"</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>;Create a new User</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>;Check the edit fuction of Action.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>140</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3876,6 +3948,7 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -3905,6 +3978,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4808,16 +4882,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O67"/>
+  <dimension ref="A1:O138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="E112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F136" sqref="F136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="2" width="29" customWidth="1"/>
-    <col min="4" max="4" width="6.125" customWidth="1"/>
+    <col min="4" max="4" width="30.5" customWidth="1"/>
     <col min="5" max="5" width="32.375" customWidth="1"/>
     <col min="6" max="6" width="59.625" customWidth="1"/>
     <col min="7" max="7" width="23.25" customWidth="1"/>
@@ -4826,12 +4900,12 @@
     <col min="10" max="10" width="26.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>839</v>
+        <v>831</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>840</v>
+        <v>832</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>757</v>
@@ -4871,12 +4945,12 @@
       </c>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:15" ht="15">
+    <row r="2" spans="1:15" ht="13.5" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>841</v>
+        <v>833</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>842</v>
+        <v>834</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
@@ -4896,12 +4970,12 @@
       <c r="N2" s="7"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" ht="13.5" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>843</v>
+        <v>835</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>844</v>
+        <v>836</v>
       </c>
       <c r="C3" s="5">
         <v>2</v>
@@ -4931,12 +5005,12 @@
       <c r="N3" s="7"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" ht="13.5" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>845</v>
+        <v>837</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>846</v>
+        <v>838</v>
       </c>
       <c r="C4" s="5">
         <v>3</v>
@@ -4962,9 +5036,9 @@
       <c r="N4" s="7"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" ht="15">
+    <row r="5" spans="1:15" ht="13.5" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>847</v>
+        <v>839</v>
       </c>
       <c r="B5" s="10">
         <v>41116</v>
@@ -4973,7 +5047,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -4984,12 +5058,12 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="7"/>
+      <c r="N5" s="16"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" ht="13.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>848</v>
+        <v>840</v>
       </c>
       <c r="B6" s="10">
         <v>41116</v>
@@ -4997,119 +5071,119 @@
       <c r="C6" s="5">
         <v>5</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>786</v>
-      </c>
-      <c r="E6" s="11" t="s">
+      <c r="D6" s="8" t="s">
+        <v>845</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>797</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="11"/>
+      <c r="F6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
-      <c r="N6" s="17"/>
+      <c r="N6" s="16"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" ht="13.5" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>765</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>853</v>
+        <v>876</v>
       </c>
       <c r="C7" s="5">
         <v>6</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>786</v>
-      </c>
-      <c r="E7" s="11" t="s">
+      <c r="D7" s="8" t="s">
+        <v>845</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="11"/>
+      <c r="G7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="N7" s="17"/>
+      <c r="N7" s="16"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" ht="13.5" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>850</v>
+        <v>842</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="5">
         <v>7</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>786</v>
+      <c r="D8" s="8" t="s">
+        <v>845</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>798</v>
-      </c>
-      <c r="H8" s="11"/>
+      <c r="F8" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>844</v>
+      </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="N8" s="17"/>
+      <c r="N8" s="16"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" ht="13.5" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>851</v>
+        <v>843</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="5">
         <v>8</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>786</v>
+      <c r="D9" s="8" t="s">
+        <v>845</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>800</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>801</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="11"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="N9" s="17"/>
+      <c r="N9" s="16"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" ht="13.5" customHeight="1">
       <c r="A10" s="13" t="s">
         <v>766</v>
       </c>
@@ -5119,59 +5193,55 @@
       <c r="C10" s="5">
         <v>9</v>
       </c>
-      <c r="D10" s="18" t="s">
-        <v>786</v>
+      <c r="D10" s="8" t="s">
+        <v>845</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>800</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>802</v>
-      </c>
-      <c r="I10" s="5"/>
+        <v>278</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
-      <c r="N10" s="17"/>
+      <c r="N10" s="16"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" ht="13.5" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="15"/>
       <c r="C11" s="5">
         <v>10</v>
       </c>
-      <c r="D11" s="18" t="s">
-        <v>786</v>
+      <c r="D11" s="8" t="s">
+        <v>845</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>800</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>803</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H11" s="11"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
-      <c r="N11" s="17"/>
+      <c r="N11" s="16"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" ht="13.5" customHeight="1">
       <c r="A12" s="23" t="s">
         <v>768</v>
       </c>
@@ -5179,30 +5249,28 @@
       <c r="C12" s="5">
         <v>11</v>
       </c>
-      <c r="D12" s="18" t="s">
-        <v>786</v>
+      <c r="D12" s="8" t="s">
+        <v>845</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>800</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>804</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H12" s="11"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
-      <c r="N12" s="17"/>
+      <c r="N12" s="16"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" ht="13.5" customHeight="1">
       <c r="A13" s="23" t="s">
         <v>769</v>
       </c>
@@ -5210,30 +5278,30 @@
       <c r="C13" s="5">
         <v>12</v>
       </c>
-      <c r="D13" s="18" t="s">
-        <v>786</v>
+      <c r="D13" s="8" t="s">
+        <v>845</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>800</v>
+        <v>278</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>804</v>
+        <v>846</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
-      <c r="N13" s="17"/>
+      <c r="N13" s="16"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" ht="13.5" customHeight="1">
       <c r="A14" s="23" t="s">
         <v>770</v>
       </c>
@@ -5241,30 +5309,28 @@
       <c r="C14" s="5">
         <v>13</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="8" t="s">
         <v>786</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>800</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>805</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="11"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
-      <c r="N14" s="17"/>
+      <c r="N14" s="16"/>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" ht="13.5" customHeight="1">
       <c r="A15" s="23" t="s">
         <v>771</v>
       </c>
@@ -5272,30 +5338,28 @@
       <c r="C15" s="5">
         <v>14</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="8" t="s">
         <v>786</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>800</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>806</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="11"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
-      <c r="N15" s="17"/>
+      <c r="N15" s="16"/>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" ht="13.5" customHeight="1">
       <c r="A16" s="23" t="s">
         <v>772</v>
       </c>
@@ -5303,30 +5367,30 @@
       <c r="C16" s="5">
         <v>15</v>
       </c>
-      <c r="D16" s="18" t="s">
-        <v>786</v>
+      <c r="D16" s="8" t="s">
+        <v>845</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>800</v>
+        <v>278</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>807</v>
-      </c>
-      <c r="I16" s="5"/>
+        <v>847</v>
+      </c>
+      <c r="I16" s="11"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
-      <c r="N16" s="17"/>
+      <c r="N16" s="16"/>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" ht="13.5" customHeight="1">
       <c r="A17" s="23" t="s">
         <v>773</v>
       </c>
@@ -5334,30 +5398,30 @@
       <c r="C17" s="5">
         <v>16</v>
       </c>
-      <c r="D17" s="18" t="s">
-        <v>786</v>
+      <c r="D17" s="8" t="s">
+        <v>845</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>800</v>
+        <v>278</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>808</v>
-      </c>
-      <c r="I17" s="5"/>
+        <v>848</v>
+      </c>
+      <c r="I17" s="11"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
-      <c r="N17" s="17"/>
+      <c r="N17" s="16"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" ht="13.5" customHeight="1">
       <c r="A18" s="23"/>
       <c r="B18" s="24" t="s">
         <v>774</v>
@@ -5365,30 +5429,28 @@
       <c r="C18" s="5">
         <v>17</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="8" t="s">
         <v>786</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>800</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>809</v>
-      </c>
-      <c r="I18" s="5"/>
+        <v>278</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
-      <c r="N18" s="17"/>
+      <c r="N18" s="16"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" ht="13.5" customHeight="1">
       <c r="A19" s="23"/>
       <c r="B19" s="24" t="s">
         <v>775</v>
@@ -5396,34 +5458,28 @@
       <c r="C19" s="5">
         <v>18</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>786</v>
+      <c r="D19" s="8" t="s">
+        <v>845</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>263</v>
+        <v>278</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>301</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>810</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>811</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>812</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>813</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
-      <c r="N19" s="17"/>
+      <c r="N19" s="16"/>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" ht="13.5" customHeight="1">
       <c r="A20" s="23" t="s">
         <v>776</v>
       </c>
@@ -5433,30 +5489,28 @@
       <c r="C20" s="5">
         <v>19</v>
       </c>
-      <c r="D20" s="18" t="s">
-        <v>814</v>
+      <c r="D20" s="8" t="s">
+        <v>845</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>263</v>
+        <v>278</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>815</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="H20" s="11"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
-      <c r="N20" s="17"/>
+      <c r="N20" s="16"/>
       <c r="O20" s="2"/>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" ht="13.5" customHeight="1">
       <c r="A21" s="23" t="s">
         <v>777</v>
       </c>
@@ -5464,30 +5518,28 @@
       <c r="C21" s="5">
         <v>20</v>
       </c>
-      <c r="D21" s="18" t="s">
-        <v>786</v>
+      <c r="D21" s="8" t="s">
+        <v>845</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>264</v>
+        <v>278</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>280</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>816</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="H21" s="11"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
-      <c r="N21" s="17"/>
+      <c r="N21" s="16"/>
       <c r="O21" s="2"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" ht="13.5" customHeight="1">
       <c r="A22" s="23" t="s">
         <v>778</v>
       </c>
@@ -5495,17 +5547,17 @@
       <c r="C22" s="5">
         <v>21</v>
       </c>
-      <c r="D22" s="18" t="s">
-        <v>786</v>
+      <c r="D22" s="8" t="s">
+        <v>845</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>265</v>
+        <v>278</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>281</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="5"/>
@@ -5513,24 +5565,24 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
-      <c r="N22" s="17"/>
+      <c r="N22" s="16"/>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" ht="13.5" customHeight="1">
       <c r="C23" s="5">
         <v>22</v>
       </c>
-      <c r="D23" s="18" t="s">
-        <v>786</v>
+      <c r="D23" s="8" t="s">
+        <v>845</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>266</v>
+        <v>278</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>282</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="5"/>
@@ -5538,24 +5590,24 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
-      <c r="N23" s="17"/>
+      <c r="N23" s="16"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" ht="13.5" customHeight="1">
       <c r="C24" s="5">
         <v>23</v>
       </c>
-      <c r="D24" s="18" t="s">
-        <v>786</v>
+      <c r="D24" s="8" t="s">
+        <v>845</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>267</v>
+        <v>278</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>283</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="5"/>
@@ -5563,24 +5615,24 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
-      <c r="N24" s="17"/>
+      <c r="N24" s="16"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" ht="13.5" customHeight="1">
       <c r="C25" s="5">
         <v>24</v>
       </c>
-      <c r="D25" s="18" t="s">
-        <v>786</v>
+      <c r="D25" s="8" t="s">
+        <v>845</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>268</v>
+        <v>278</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>284</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H25" s="11"/>
       <c r="I25" s="5"/>
@@ -5588,24 +5640,24 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
-      <c r="N25" s="17"/>
+      <c r="N25" s="16"/>
       <c r="O25" s="2"/>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" ht="13.5" customHeight="1">
       <c r="C26" s="5">
         <v>25</v>
       </c>
-      <c r="D26" s="18" t="s">
-        <v>786</v>
+      <c r="D26" s="8" t="s">
+        <v>845</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>269</v>
+        <v>278</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>285</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H26" s="11"/>
       <c r="I26" s="5"/>
@@ -5613,24 +5665,24 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
-      <c r="N26" s="17"/>
+      <c r="N26" s="16"/>
       <c r="O26" s="2"/>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" ht="13.5" customHeight="1">
       <c r="C27" s="5">
         <v>26</v>
       </c>
-      <c r="D27" s="18" t="s">
-        <v>814</v>
+      <c r="D27" s="8" t="s">
+        <v>845</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>270</v>
+        <v>278</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>286</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>798</v>
+        <v>142</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="5"/>
@@ -5638,69 +5690,69 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
-      <c r="N27" s="17"/>
+      <c r="N27" s="16"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" ht="13.5" customHeight="1">
       <c r="C28" s="5">
         <v>27</v>
       </c>
-      <c r="D28" s="18" t="s">
+      <c r="D28" s="8" t="s">
         <v>786</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>817</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>798</v>
+        <v>278</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="H28" s="11"/>
-      <c r="I28" s="5"/>
+      <c r="I28" s="11"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
-      <c r="N28" s="17"/>
+      <c r="N28" s="16"/>
       <c r="O28" s="2"/>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" ht="13.5" customHeight="1">
       <c r="C29" s="5">
         <v>28</v>
       </c>
-      <c r="D29" s="18" t="s">
-        <v>786</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>818</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>819</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>798</v>
-      </c>
-      <c r="H29" s="11"/>
+      <c r="D29" s="6" t="s">
+        <v>874</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
-      <c r="N29" s="17"/>
+      <c r="N29" s="7"/>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" spans="1:15" ht="15">
+    <row r="30" spans="1:15" ht="13.5" customHeight="1">
       <c r="C30" s="5">
         <v>29</v>
       </c>
-      <c r="D30" s="19" t="s">
-        <v>820</v>
-      </c>
-      <c r="E30" s="20"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
+      <c r="D30" s="18" t="s">
+        <v>786</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>796</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="H30" s="11"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
@@ -5710,7 +5762,7 @@
       <c r="N30" s="17"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" ht="13.5" customHeight="1">
       <c r="C31" s="5">
         <v>30</v>
       </c>
@@ -5721,7 +5773,7 @@
         <v>19</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>821</v>
+        <v>81</v>
       </c>
       <c r="G31" s="11" t="s">
         <v>2</v>
@@ -5735,7 +5787,7 @@
       <c r="N31" s="17"/>
       <c r="O31" s="2"/>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" ht="13.5" customHeight="1">
       <c r="C32" s="5">
         <v>31</v>
       </c>
@@ -5743,13 +5795,13 @@
         <v>786</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>19</v>
+        <v>241</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>74</v>
+        <v>242</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>2</v>
+        <v>797</v>
       </c>
       <c r="H32" s="11"/>
       <c r="I32" s="5"/>
@@ -5760,24 +5812,24 @@
       <c r="N32" s="17"/>
       <c r="O32" s="2"/>
     </row>
-    <row r="33" spans="3:15">
+    <row r="33" spans="3:15" ht="13.5" customHeight="1">
       <c r="C33" s="5">
         <v>32</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>822</v>
+        <v>786</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>823</v>
+        <v>798</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>1</v>
+        <v>256</v>
       </c>
       <c r="G33" s="11" t="s">
+        <v>799</v>
+      </c>
+      <c r="H33" s="11" t="s">
         <v>800</v>
-      </c>
-      <c r="H33" s="11" t="s">
-        <v>801</v>
       </c>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
@@ -5792,19 +5844,19 @@
         <v>33</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>822</v>
+        <v>786</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>823</v>
+        <v>798</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>9</v>
+        <v>258</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
@@ -5819,19 +5871,19 @@
         <v>34</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>822</v>
+        <v>786</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>823</v>
+        <v>798</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>12</v>
+        <v>255</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>824</v>
+        <v>802</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
@@ -5846,18 +5898,20 @@
         <v>35</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>822</v>
+        <v>786</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>823</v>
+        <v>798</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>798</v>
-      </c>
-      <c r="H36" s="11"/>
+        <v>799</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>803</v>
+      </c>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
@@ -5871,24 +5925,26 @@
         <v>36</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>838</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H37" s="5"/>
+        <v>786</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>798</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>799</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>803</v>
+      </c>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
       <c r="M37" s="5"/>
-      <c r="N37" s="7"/>
+      <c r="N37" s="17"/>
       <c r="O37" s="2"/>
     </row>
     <row r="38" spans="3:15">
@@ -5896,217 +5952,230 @@
         <v>37</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>794</v>
+        <v>786</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>796</v>
-      </c>
-      <c r="F38" s="11">
-        <v>5</v>
-      </c>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
+        <v>798</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>799</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>804</v>
+      </c>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
       <c r="N38" s="17"/>
+      <c r="O38" s="2"/>
     </row>
-    <row r="39" spans="3:15" ht="15">
+    <row r="39" spans="3:15">
       <c r="C39" s="5">
         <v>38</v>
       </c>
-      <c r="D39" s="19" t="s">
-        <v>825</v>
-      </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="11"/>
+      <c r="D39" s="18" t="s">
+        <v>786</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>798</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>799</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>805</v>
+      </c>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
       <c r="M39" s="5"/>
-      <c r="N39" s="16"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="2"/>
     </row>
     <row r="40" spans="3:15">
       <c r="C40" s="5">
         <v>39</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="18" t="s">
         <v>786</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
+        <v>798</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>799</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>806</v>
+      </c>
+      <c r="I40" s="5"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
       <c r="M40" s="5"/>
-      <c r="N40" s="16"/>
+      <c r="N40" s="17"/>
+      <c r="O40" s="2"/>
     </row>
     <row r="41" spans="3:15">
       <c r="C41" s="5">
         <v>40</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="18" t="s">
         <v>786</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H41" s="5"/>
-      <c r="I41" s="11"/>
+        <v>798</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>799</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>807</v>
+      </c>
+      <c r="I41" s="5"/>
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
       <c r="M41" s="5"/>
-      <c r="N41" s="16"/>
+      <c r="N41" s="17"/>
       <c r="O41" s="2"/>
     </row>
     <row r="42" spans="3:15">
       <c r="C42" s="5">
         <v>41</v>
       </c>
-      <c r="D42" s="8" t="s">
-        <v>786</v>
+      <c r="D42" s="18" t="s">
+        <v>850</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H42" s="11"/>
+        <v>798</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>799</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>808</v>
+      </c>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
-      <c r="N42" s="16"/>
+      <c r="N42" s="17"/>
       <c r="O42" s="2"/>
     </row>
     <row r="43" spans="3:15">
       <c r="C43" s="5">
         <v>42</v>
       </c>
-      <c r="D43" s="8" t="s">
-        <v>786</v>
+      <c r="D43" s="18" t="s">
+        <v>851</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>310</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H43" s="11"/>
+        <v>798</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>847</v>
+      </c>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
       <c r="M43" s="5"/>
-      <c r="N43" s="16"/>
+      <c r="N43" s="17"/>
       <c r="O43" s="2"/>
     </row>
     <row r="44" spans="3:15">
       <c r="C44" s="5">
         <v>43</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="18" t="s">
         <v>786</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>7</v>
+        <v>798</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>827</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>787</v>
-      </c>
-      <c r="J44" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>810</v>
+      </c>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
       <c r="M44" s="5"/>
-      <c r="N44" s="16"/>
+      <c r="N44" s="17"/>
       <c r="O44" s="2"/>
     </row>
     <row r="45" spans="3:15">
       <c r="C45" s="5">
         <v>44</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="18" t="s">
         <v>786</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H45" s="11" t="s">
-        <v>827</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>787</v>
-      </c>
-      <c r="J45" s="5" t="b">
-        <v>0</v>
-      </c>
+        <v>798</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="H45" s="11"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
       <c r="M45" s="5"/>
-      <c r="N45" s="16"/>
+      <c r="N45" s="17"/>
       <c r="O45" s="2"/>
     </row>
     <row r="46" spans="3:15">
       <c r="C46" s="5">
         <v>45</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="18" t="s">
         <v>786</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>2</v>
+        <v>798</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>143</v>
       </c>
       <c r="H46" s="11"/>
       <c r="I46" s="5"/>
@@ -6114,24 +6183,24 @@
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
       <c r="M46" s="5"/>
-      <c r="N46" s="16"/>
+      <c r="N46" s="17"/>
       <c r="O46" s="2"/>
     </row>
     <row r="47" spans="3:15">
       <c r="C47" s="5">
         <v>46</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="18" t="s">
         <v>786</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>310</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>2</v>
+        <v>798</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>143</v>
       </c>
       <c r="H47" s="11"/>
       <c r="I47" s="5"/>
@@ -6139,24 +6208,24 @@
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
       <c r="M47" s="5"/>
-      <c r="N47" s="16"/>
+      <c r="N47" s="17"/>
       <c r="O47" s="2"/>
     </row>
     <row r="48" spans="3:15">
       <c r="C48" s="5">
         <v>47</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="18" t="s">
         <v>786</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>2</v>
+        <v>798</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>143</v>
       </c>
       <c r="H48" s="11"/>
       <c r="I48" s="5"/>
@@ -6164,43 +6233,49 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
-      <c r="N48" s="16"/>
+      <c r="N48" s="17"/>
       <c r="O48" s="2"/>
     </row>
-    <row r="49" spans="3:15" ht="15">
+    <row r="49" spans="3:15">
       <c r="C49" s="5">
         <v>48</v>
       </c>
-      <c r="D49" s="19" t="s">
-        <v>828</v>
-      </c>
-      <c r="E49" s="20"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
+      <c r="D49" s="18" t="s">
+        <v>786</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>798</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>143</v>
+      </c>
       <c r="H49" s="11"/>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
       <c r="M49" s="5"/>
-      <c r="N49" s="21"/>
-      <c r="O49" s="22"/>
+      <c r="N49" s="17"/>
+      <c r="O49" s="2"/>
     </row>
     <row r="50" spans="3:15">
       <c r="C50" s="5">
         <v>49</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>786</v>
+        <v>809</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>19</v>
+        <v>798</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>829</v>
+        <v>270</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>2</v>
+        <v>797</v>
       </c>
       <c r="H50" s="11"/>
       <c r="I50" s="5"/>
@@ -6208,8 +6283,8 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
       <c r="M50" s="5"/>
-      <c r="N50" s="21"/>
-      <c r="O50" s="22"/>
+      <c r="N50" s="17"/>
+      <c r="O50" s="2"/>
     </row>
     <row r="51" spans="3:15">
       <c r="C51" s="5">
@@ -6219,13 +6294,13 @@
         <v>786</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>19</v>
+        <v>798</v>
       </c>
       <c r="F51" s="11" t="s">
-        <v>74</v>
+        <v>811</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>2</v>
+        <v>797</v>
       </c>
       <c r="H51" s="11"/>
       <c r="I51" s="5"/>
@@ -6233,105 +6308,93 @@
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
       <c r="M51" s="5"/>
-      <c r="N51" s="21"/>
-      <c r="O51" s="22"/>
+      <c r="N51" s="17"/>
+      <c r="O51" s="2"/>
     </row>
     <row r="52" spans="3:15">
       <c r="C52" s="5">
         <v>51</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>830</v>
+        <v>786</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>831</v>
+        <v>812</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>1</v>
+        <v>813</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>832</v>
-      </c>
-      <c r="H52" s="11" t="s">
-        <v>833</v>
-      </c>
+        <v>797</v>
+      </c>
+      <c r="H52" s="11"/>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
       <c r="M52" s="5"/>
-      <c r="N52" s="21"/>
-      <c r="O52" s="22"/>
+      <c r="N52" s="17"/>
+      <c r="O52" s="2"/>
     </row>
-    <row r="53" spans="3:15">
+    <row r="53" spans="3:15" ht="15">
       <c r="C53" s="5">
         <v>52</v>
       </c>
-      <c r="D53" s="18" t="s">
-        <v>830</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>831</v>
-      </c>
-      <c r="F53" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G53" s="11" t="s">
-        <v>832</v>
-      </c>
-      <c r="H53" s="11" t="s">
-        <v>834</v>
-      </c>
+      <c r="D53" s="19" t="s">
+        <v>814</v>
+      </c>
+      <c r="E53" s="20"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
       <c r="M53" s="5"/>
-      <c r="N53" s="21"/>
-      <c r="O53" s="22"/>
+      <c r="N53" s="17"/>
+      <c r="O53" s="2"/>
     </row>
     <row r="54" spans="3:15">
       <c r="C54" s="5">
         <v>53</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>830</v>
+        <v>786</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>831</v>
+        <v>19</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>12</v>
+        <v>815</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>832</v>
-      </c>
-      <c r="H54" s="11" t="s">
-        <v>835</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H54" s="11"/>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
       <c r="M54" s="5"/>
-      <c r="N54" s="21"/>
-      <c r="O54" s="22"/>
+      <c r="N54" s="17"/>
+      <c r="O54" s="2"/>
     </row>
     <row r="55" spans="3:15">
       <c r="C55" s="5">
         <v>54</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>830</v>
+        <v>786</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>831</v>
+        <v>19</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>836</v>
+        <v>74</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>837</v>
+        <v>2</v>
       </c>
       <c r="H55" s="11"/>
       <c r="I55" s="5"/>
@@ -6339,113 +6402,127 @@
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
       <c r="M55" s="5"/>
-      <c r="N55" s="21"/>
-      <c r="O55" s="22"/>
+      <c r="N55" s="17"/>
+      <c r="O55" s="2"/>
     </row>
-    <row r="56" spans="3:15" ht="15">
+    <row r="56" spans="3:15">
       <c r="C56" s="5">
         <v>55</v>
       </c>
-      <c r="D56" s="6" t="s">
-        <v>784</v>
-      </c>
-      <c r="E56" s="11"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11"/>
+      <c r="D56" s="18" t="s">
+        <v>816</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>817</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>799</v>
+      </c>
+      <c r="H56" s="11" t="s">
+        <v>800</v>
+      </c>
+      <c r="I56" s="5"/>
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
       <c r="M56" s="5"/>
-      <c r="N56" s="7"/>
+      <c r="N56" s="17"/>
+      <c r="O56" s="2"/>
     </row>
     <row r="57" spans="3:15">
       <c r="C57" s="5">
         <v>56</v>
       </c>
-      <c r="D57" s="8" t="s">
-        <v>790</v>
+      <c r="D57" s="18" t="s">
+        <v>816</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>791</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>792</v>
-      </c>
-      <c r="H57" s="5"/>
-      <c r="I57" s="11"/>
+        <v>817</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>799</v>
+      </c>
+      <c r="H57" s="11" t="s">
+        <v>852</v>
+      </c>
+      <c r="I57" s="5"/>
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
       <c r="M57" s="5"/>
       <c r="N57" s="17"/>
+      <c r="O57" s="2"/>
     </row>
     <row r="58" spans="3:15">
       <c r="C58" s="5">
         <v>57</v>
       </c>
-      <c r="D58" s="8" t="s">
-        <v>790</v>
+      <c r="D58" s="18" t="s">
+        <v>816</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G58" s="5" t="s">
-        <v>792</v>
-      </c>
-      <c r="H58" s="11"/>
+        <v>817</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>799</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>818</v>
+      </c>
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
       <c r="M58" s="5"/>
-      <c r="N58" s="16"/>
+      <c r="N58" s="17"/>
+      <c r="O58" s="2"/>
     </row>
     <row r="59" spans="3:15">
       <c r="C59" s="5">
         <v>58</v>
       </c>
-      <c r="D59" s="8" t="s">
-        <v>790</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H59" s="5" t="s">
-        <v>793</v>
-      </c>
-      <c r="I59" s="11"/>
+      <c r="D59" s="18" t="s">
+        <v>816</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>817</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>797</v>
+      </c>
+      <c r="H59" s="11"/>
+      <c r="I59" s="5"/>
       <c r="J59" s="5"/>
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
       <c r="M59" s="5"/>
       <c r="N59" s="17"/>
+      <c r="O59" s="2"/>
     </row>
     <row r="60" spans="3:15">
       <c r="C60" s="5">
         <v>59</v>
       </c>
-      <c r="D60" s="8" t="s">
-        <v>790</v>
+      <c r="D60" s="18" t="s">
+        <v>830</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>241</v>
+        <v>18</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>250</v>
+        <v>17</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>2</v>
@@ -6456,47 +6533,42 @@
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
       <c r="M60" s="5"/>
-      <c r="N60" s="16"/>
+      <c r="N60" s="7"/>
+      <c r="O60" s="2"/>
     </row>
     <row r="61" spans="3:15">
       <c r="C61" s="5">
         <v>60</v>
       </c>
-      <c r="D61" s="8" t="s">
-        <v>790</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H61" s="5"/>
+      <c r="D61" s="18" t="s">
+        <v>793</v>
+      </c>
+      <c r="E61" s="11" t="s">
+        <v>795</v>
+      </c>
+      <c r="F61" s="11">
+        <v>5</v>
+      </c>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
       <c r="M61" s="5"/>
-      <c r="N61" s="16"/>
+      <c r="N61" s="17"/>
     </row>
-    <row r="62" spans="3:15">
+    <row r="62" spans="3:15" ht="15">
       <c r="C62" s="5">
         <v>61</v>
       </c>
-      <c r="D62" s="8" t="s">
-        <v>826</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>795</v>
-      </c>
-      <c r="F62" s="5">
-        <v>2</v>
-      </c>
+      <c r="D62" s="19" t="s">
+        <v>875</v>
+      </c>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
       <c r="G62" s="5"/>
-      <c r="H62" s="5"/>
+      <c r="H62" s="11"/>
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
@@ -6509,19 +6581,19 @@
         <v>62</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>790</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>278</v>
+        <v>786</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="11"/>
       <c r="J63" s="5"/>
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
@@ -6533,124 +6605,1995 @@
         <v>63</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>790</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>241</v>
+        <v>786</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>252</v>
+        <v>79</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H64" s="11" t="s">
-        <v>801</v>
-      </c>
-      <c r="I64" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="H64" s="5"/>
+      <c r="I64" s="11"/>
       <c r="J64" s="5"/>
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
       <c r="M64" s="5"/>
-      <c r="N64" s="17"/>
+      <c r="N64" s="16"/>
+      <c r="O64" s="2"/>
     </row>
-    <row r="65" spans="3:14">
+    <row r="65" spans="3:15">
       <c r="C65" s="5">
         <v>64</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>790</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>241</v>
+        <v>786</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>306</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>245</v>
+        <v>183</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H65" s="5"/>
+      <c r="H65" s="11"/>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
       <c r="M65" s="5"/>
-      <c r="N65" s="17"/>
+      <c r="N65" s="16"/>
+      <c r="O65" s="2"/>
     </row>
-    <row r="66" spans="3:14">
+    <row r="66" spans="3:15">
       <c r="C66" s="5">
         <v>65</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>790</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>241</v>
+        <v>786</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>310</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>99</v>
+        <v>256</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H66" s="11"/>
+        <v>4</v>
+      </c>
+      <c r="H66" s="11" t="s">
+        <v>871</v>
+      </c>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
       <c r="M66" s="5"/>
       <c r="N66" s="16"/>
+      <c r="O66" s="2"/>
     </row>
-    <row r="67" spans="3:14">
+    <row r="67" spans="3:15">
       <c r="C67" s="5">
         <v>66</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>826</v>
+        <v>786</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>795</v>
-      </c>
-      <c r="F67" s="5">
-        <v>2</v>
-      </c>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
+        <v>310</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>872</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H67" s="11" t="s">
+        <v>873</v>
+      </c>
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
       <c r="M67" s="5"/>
       <c r="N67" s="16"/>
+      <c r="O67" s="2"/>
+    </row>
+    <row r="68" spans="3:15">
+      <c r="C68" s="5">
+        <v>67</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E68" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H68" s="11"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="16"/>
+      <c r="O68" s="2"/>
+    </row>
+    <row r="69" spans="3:15">
+      <c r="C69" s="5">
+        <v>68</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H69" s="11" t="s">
+        <v>820</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="J69" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="16"/>
+      <c r="O69" s="2"/>
+    </row>
+    <row r="70" spans="3:15">
+      <c r="C70" s="5">
+        <v>69</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H70" s="11" t="s">
+        <v>820</v>
+      </c>
+      <c r="I70" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="J70" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="16"/>
+      <c r="O70" s="2"/>
+    </row>
+    <row r="71" spans="3:15">
+      <c r="C71" s="5">
+        <v>70</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E71" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H71" s="11" t="s">
+        <v>820</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="J71" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K71" s="5"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="5"/>
+      <c r="N71" s="16"/>
+      <c r="O71" s="2"/>
+    </row>
+    <row r="72" spans="3:15">
+      <c r="C72" s="5">
+        <v>71</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E72" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H72" s="11" t="s">
+        <v>820</v>
+      </c>
+      <c r="I72" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="J72" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K72" s="5"/>
+      <c r="L72" s="5"/>
+      <c r="M72" s="5"/>
+      <c r="N72" s="16"/>
+      <c r="O72" s="2"/>
+    </row>
+    <row r="73" spans="3:15">
+      <c r="C73" s="5">
+        <v>72</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E73" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H73" s="11" t="s">
+        <v>820</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="J73" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K73" s="5"/>
+      <c r="L73" s="5"/>
+      <c r="M73" s="5"/>
+      <c r="N73" s="16"/>
+      <c r="O73" s="2"/>
+    </row>
+    <row r="74" spans="3:15">
+      <c r="C74" s="5">
+        <v>73</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E74" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H74" s="11" t="s">
+        <v>820</v>
+      </c>
+      <c r="I74" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="J74" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K74" s="5"/>
+      <c r="L74" s="5"/>
+      <c r="M74" s="5"/>
+      <c r="N74" s="16"/>
+      <c r="O74" s="2"/>
+    </row>
+    <row r="75" spans="3:15">
+      <c r="C75" s="5">
+        <v>74</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H75" s="11" t="s">
+        <v>820</v>
+      </c>
+      <c r="I75" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="J75" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K75" s="5"/>
+      <c r="L75" s="5"/>
+      <c r="M75" s="5"/>
+      <c r="N75" s="16"/>
+      <c r="O75" s="2"/>
+    </row>
+    <row r="76" spans="3:15">
+      <c r="C76" s="5">
+        <v>75</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>870</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H76" s="11"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5"/>
+      <c r="L76" s="5"/>
+      <c r="M76" s="5"/>
+      <c r="N76" s="16"/>
+      <c r="O76" s="2"/>
+    </row>
+    <row r="77" spans="3:15">
+      <c r="C77" s="5">
+        <v>76</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>870</v>
+      </c>
+      <c r="E77" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H77" s="11"/>
+      <c r="I77" s="5"/>
+      <c r="J77" s="5"/>
+      <c r="K77" s="5"/>
+      <c r="L77" s="5"/>
+      <c r="M77" s="5"/>
+      <c r="N77" s="16"/>
+      <c r="O77" s="2"/>
+    </row>
+    <row r="78" spans="3:15">
+      <c r="C78" s="5">
+        <v>77</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>870</v>
+      </c>
+      <c r="E78" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H78" s="11"/>
+      <c r="I78" s="5"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="5"/>
+      <c r="L78" s="5"/>
+      <c r="M78" s="5"/>
+      <c r="N78" s="16"/>
+      <c r="O78" s="2"/>
+    </row>
+    <row r="79" spans="3:15">
+      <c r="C79" s="5">
+        <v>78</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H79" s="11"/>
+      <c r="I79" s="5"/>
+      <c r="J79" s="5"/>
+      <c r="K79" s="5"/>
+      <c r="L79" s="5"/>
+      <c r="M79" s="5"/>
+      <c r="N79" s="16"/>
+      <c r="O79" s="2"/>
+    </row>
+    <row r="80" spans="3:15">
+      <c r="C80" s="5">
+        <v>79</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E80" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H80" s="11"/>
+      <c r="I80" s="5"/>
+      <c r="J80" s="5"/>
+      <c r="K80" s="5"/>
+      <c r="L80" s="5"/>
+      <c r="M80" s="5"/>
+      <c r="N80" s="16"/>
+      <c r="O80" s="2"/>
+    </row>
+    <row r="81" spans="3:15">
+      <c r="C81" s="5">
+        <v>80</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E81" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H81" s="11" t="s">
+        <v>853</v>
+      </c>
+      <c r="I81" s="11"/>
+      <c r="J81" s="5"/>
+      <c r="K81" s="5"/>
+      <c r="L81" s="5"/>
+      <c r="M81" s="5"/>
+      <c r="N81" s="16"/>
+      <c r="O81" s="2"/>
+    </row>
+    <row r="82" spans="3:15">
+      <c r="C82" s="5">
+        <v>81</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E82" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H82" s="11" t="s">
+        <v>854</v>
+      </c>
+      <c r="I82" s="11"/>
+      <c r="J82" s="5"/>
+      <c r="K82" s="5"/>
+      <c r="L82" s="5"/>
+      <c r="M82" s="5"/>
+      <c r="N82" s="16"/>
+      <c r="O82" s="2"/>
+    </row>
+    <row r="83" spans="3:15">
+      <c r="C83" s="5">
+        <v>82</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E83" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H83" s="11" t="s">
+        <v>855</v>
+      </c>
+      <c r="I83" s="11"/>
+      <c r="J83" s="5"/>
+      <c r="K83" s="5"/>
+      <c r="L83" s="5"/>
+      <c r="M83" s="5"/>
+      <c r="N83" s="16"/>
+      <c r="O83" s="2"/>
+    </row>
+    <row r="84" spans="3:15">
+      <c r="C84" s="5">
+        <v>83</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E84" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H84" s="11"/>
+      <c r="I84" s="11"/>
+      <c r="J84" s="5"/>
+      <c r="K84" s="5"/>
+      <c r="L84" s="5"/>
+      <c r="M84" s="5"/>
+      <c r="N84" s="16"/>
+      <c r="O84" s="2"/>
+    </row>
+    <row r="85" spans="3:15">
+      <c r="C85" s="5">
+        <v>84</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E85" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H85" s="11" t="s">
+        <v>856</v>
+      </c>
+      <c r="I85" s="5"/>
+      <c r="J85" s="5"/>
+      <c r="K85" s="5"/>
+      <c r="L85" s="5"/>
+      <c r="M85" s="5"/>
+      <c r="N85" s="16"/>
+      <c r="O85" s="2"/>
+    </row>
+    <row r="86" spans="3:15">
+      <c r="C86" s="5">
+        <v>85</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E86" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="G86" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H86" s="11" t="s">
+        <v>857</v>
+      </c>
+      <c r="I86" s="5"/>
+      <c r="J86" s="5"/>
+      <c r="K86" s="5"/>
+      <c r="L86" s="5"/>
+      <c r="M86" s="5"/>
+      <c r="N86" s="16"/>
+      <c r="O86" s="2"/>
+    </row>
+    <row r="87" spans="3:15">
+      <c r="C87" s="5">
+        <v>86</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E87" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="G87" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H87" s="11"/>
+      <c r="I87" s="11"/>
+      <c r="J87" s="5"/>
+      <c r="K87" s="5"/>
+      <c r="L87" s="5"/>
+      <c r="M87" s="5"/>
+      <c r="N87" s="16"/>
+      <c r="O87" s="2"/>
+    </row>
+    <row r="88" spans="3:15">
+      <c r="C88" s="5">
+        <v>87</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E88" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H88" s="11"/>
+      <c r="I88" s="5"/>
+      <c r="J88" s="5"/>
+      <c r="K88" s="5"/>
+      <c r="L88" s="5"/>
+      <c r="M88" s="5"/>
+      <c r="N88" s="16"/>
+      <c r="O88" s="2"/>
+    </row>
+    <row r="89" spans="3:15">
+      <c r="C89" s="5">
+        <v>88</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E89" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H89" s="11" t="s">
+        <v>858</v>
+      </c>
+      <c r="I89" s="11"/>
+      <c r="J89" s="5"/>
+      <c r="K89" s="5"/>
+      <c r="L89" s="5"/>
+      <c r="M89" s="5"/>
+      <c r="N89" s="16"/>
+      <c r="O89" s="2"/>
+    </row>
+    <row r="90" spans="3:15">
+      <c r="C90" s="5">
+        <v>89</v>
+      </c>
+      <c r="D90" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E90" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="G90" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H90" s="11" t="s">
+        <v>859</v>
+      </c>
+      <c r="I90" s="5"/>
+      <c r="J90" s="5"/>
+      <c r="K90" s="5"/>
+      <c r="L90" s="5"/>
+      <c r="M90" s="5"/>
+      <c r="N90" s="16"/>
+      <c r="O90" s="2"/>
+    </row>
+    <row r="91" spans="3:15">
+      <c r="C91" s="5">
+        <v>90</v>
+      </c>
+      <c r="D91" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E91" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="G91" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H91" s="11" t="s">
+        <v>860</v>
+      </c>
+      <c r="I91" s="5"/>
+      <c r="J91" s="5"/>
+      <c r="K91" s="5"/>
+      <c r="L91" s="5"/>
+      <c r="M91" s="5"/>
+      <c r="N91" s="16"/>
+      <c r="O91" s="2"/>
+    </row>
+    <row r="92" spans="3:15">
+      <c r="C92" s="5">
+        <v>91</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E92" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="G92" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H92" s="5" t="s">
+        <v>861</v>
+      </c>
+      <c r="I92" s="5"/>
+      <c r="J92" s="5"/>
+      <c r="K92" s="5"/>
+      <c r="L92" s="5"/>
+      <c r="M92" s="5"/>
+      <c r="N92" s="16"/>
+      <c r="O92" s="2"/>
+    </row>
+    <row r="93" spans="3:15">
+      <c r="C93" s="5">
+        <v>92</v>
+      </c>
+      <c r="D93" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E93" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="G93" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H93" s="11" t="s">
+        <v>862</v>
+      </c>
+      <c r="I93" s="5"/>
+      <c r="J93" s="5"/>
+      <c r="K93" s="5"/>
+      <c r="L93" s="5"/>
+      <c r="M93" s="5"/>
+      <c r="N93" s="16"/>
+      <c r="O93" s="2"/>
+    </row>
+    <row r="94" spans="3:15">
+      <c r="C94" s="5">
+        <v>93</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E94" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="G94" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H94" s="11" t="s">
+        <v>863</v>
+      </c>
+      <c r="I94" s="5"/>
+      <c r="J94" s="5"/>
+      <c r="K94" s="5"/>
+      <c r="L94" s="5"/>
+      <c r="M94" s="5"/>
+      <c r="N94" s="16"/>
+      <c r="O94" s="2"/>
+    </row>
+    <row r="95" spans="3:15">
+      <c r="C95" s="5">
+        <v>94</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E95" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="G95" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H95" s="11"/>
+      <c r="I95" s="11"/>
+      <c r="J95" s="5"/>
+      <c r="K95" s="5"/>
+      <c r="L95" s="5"/>
+      <c r="M95" s="5"/>
+      <c r="N95" s="16"/>
+      <c r="O95" s="2"/>
+    </row>
+    <row r="96" spans="3:15">
+      <c r="C96" s="5">
+        <v>95</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E96" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="G96" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H96" s="11"/>
+      <c r="I96" s="11"/>
+      <c r="J96" s="5"/>
+      <c r="K96" s="5"/>
+      <c r="L96" s="5"/>
+      <c r="M96" s="5"/>
+      <c r="N96" s="16"/>
+      <c r="O96" s="2"/>
+    </row>
+    <row r="97" spans="3:15">
+      <c r="C97" s="5">
+        <v>96</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E97" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G97" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H97" s="11"/>
+      <c r="I97" s="11"/>
+      <c r="J97" s="5"/>
+      <c r="K97" s="5"/>
+      <c r="L97" s="5"/>
+      <c r="M97" s="5"/>
+      <c r="N97" s="16"/>
+      <c r="O97" s="2"/>
+    </row>
+    <row r="98" spans="3:15">
+      <c r="C98" s="5">
+        <v>97</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E98" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H98" s="11"/>
+      <c r="I98" s="11"/>
+      <c r="J98" s="5"/>
+      <c r="K98" s="5"/>
+      <c r="L98" s="5"/>
+      <c r="M98" s="5"/>
+      <c r="N98" s="16"/>
+      <c r="O98" s="2"/>
+    </row>
+    <row r="99" spans="3:15">
+      <c r="C99" s="5">
+        <v>98</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E99" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G99" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H99" s="11"/>
+      <c r="I99" s="11"/>
+      <c r="J99" s="5"/>
+      <c r="K99" s="5"/>
+      <c r="L99" s="5"/>
+      <c r="M99" s="5"/>
+      <c r="N99" s="16"/>
+      <c r="O99" s="2"/>
+    </row>
+    <row r="100" spans="3:15">
+      <c r="C100" s="5">
+        <v>99</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E100" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="G100" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H100" s="11" t="s">
+        <v>864</v>
+      </c>
+      <c r="I100" s="11"/>
+      <c r="J100" s="5"/>
+      <c r="K100" s="5"/>
+      <c r="L100" s="5"/>
+      <c r="M100" s="5"/>
+      <c r="N100" s="16"/>
+      <c r="O100" s="2"/>
+    </row>
+    <row r="101" spans="3:15">
+      <c r="C101" s="5">
+        <v>100</v>
+      </c>
+      <c r="D101" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E101" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G101" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H101" s="11"/>
+      <c r="I101" s="11"/>
+      <c r="J101" s="5"/>
+      <c r="K101" s="5"/>
+      <c r="L101" s="5"/>
+      <c r="M101" s="5"/>
+      <c r="N101" s="16"/>
+      <c r="O101" s="2"/>
+    </row>
+    <row r="102" spans="3:15">
+      <c r="C102" s="5">
+        <v>101</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E102" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="G102" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H102" s="11" t="s">
+        <v>853</v>
+      </c>
+      <c r="I102" s="11"/>
+      <c r="J102" s="5"/>
+      <c r="K102" s="5"/>
+      <c r="L102" s="5"/>
+      <c r="M102" s="5"/>
+      <c r="N102" s="16"/>
+      <c r="O102" s="2"/>
+    </row>
+    <row r="103" spans="3:15">
+      <c r="C103" s="5">
+        <v>102</v>
+      </c>
+      <c r="D103" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E103" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G103" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H103" s="11"/>
+      <c r="I103" s="11"/>
+      <c r="J103" s="5"/>
+      <c r="K103" s="5"/>
+      <c r="L103" s="5"/>
+      <c r="M103" s="5"/>
+      <c r="N103" s="16"/>
+      <c r="O103" s="2"/>
+    </row>
+    <row r="104" spans="3:15">
+      <c r="C104" s="5">
+        <v>103</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E104" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G104" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H104" s="11"/>
+      <c r="I104" s="11"/>
+      <c r="J104" s="5"/>
+      <c r="K104" s="5"/>
+      <c r="L104" s="5"/>
+      <c r="M104" s="5"/>
+      <c r="N104" s="16"/>
+      <c r="O104" s="2"/>
+    </row>
+    <row r="105" spans="3:15">
+      <c r="C105" s="5">
+        <v>104</v>
+      </c>
+      <c r="D105" s="8" t="s">
+        <v>865</v>
+      </c>
+      <c r="E105" s="11" t="s">
+        <v>756</v>
+      </c>
+      <c r="F105" s="5">
+        <v>2</v>
+      </c>
+      <c r="G105" s="5"/>
+      <c r="H105" s="11"/>
+      <c r="I105" s="11"/>
+      <c r="J105" s="5"/>
+      <c r="K105" s="5"/>
+      <c r="L105" s="5"/>
+      <c r="M105" s="5"/>
+      <c r="N105" s="16"/>
+      <c r="O105" s="2"/>
+    </row>
+    <row r="106" spans="3:15">
+      <c r="C106" s="5">
+        <v>105</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G106" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H106" s="5"/>
+      <c r="I106" s="5"/>
+      <c r="J106" s="5"/>
+      <c r="K106" s="5"/>
+      <c r="L106" s="5"/>
+      <c r="M106" s="5"/>
+      <c r="N106" s="16"/>
+      <c r="O106" s="2"/>
+    </row>
+    <row r="107" spans="3:15">
+      <c r="C107" s="5">
+        <v>106</v>
+      </c>
+      <c r="D107" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G107" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H107" s="5"/>
+      <c r="I107" s="5"/>
+      <c r="J107" s="5"/>
+      <c r="K107" s="5"/>
+      <c r="L107" s="5"/>
+      <c r="M107" s="5"/>
+      <c r="N107" s="16"/>
+      <c r="O107" s="2"/>
+    </row>
+    <row r="108" spans="3:15">
+      <c r="C108" s="5">
+        <v>107</v>
+      </c>
+      <c r="D108" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E108" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="G108" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H108" s="11" t="s">
+        <v>871</v>
+      </c>
+      <c r="I108" s="11"/>
+      <c r="J108" s="5"/>
+      <c r="K108" s="5"/>
+      <c r="L108" s="5"/>
+      <c r="M108" s="5"/>
+      <c r="N108" s="16"/>
+      <c r="O108" s="2"/>
+    </row>
+    <row r="109" spans="3:15">
+      <c r="C109" s="5">
+        <v>108</v>
+      </c>
+      <c r="D109" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E109" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="F109" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G109" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H109" s="11"/>
+      <c r="I109" s="11"/>
+      <c r="J109" s="5"/>
+      <c r="K109" s="5"/>
+      <c r="L109" s="5"/>
+      <c r="M109" s="5"/>
+      <c r="N109" s="16"/>
+      <c r="O109" s="2"/>
+    </row>
+    <row r="110" spans="3:15">
+      <c r="C110" s="5">
+        <v>109</v>
+      </c>
+      <c r="D110" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E110" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="F110" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="G110" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H110" s="11" t="s">
+        <v>853</v>
+      </c>
+      <c r="I110" s="11"/>
+      <c r="J110" s="5"/>
+      <c r="K110" s="5"/>
+      <c r="L110" s="5"/>
+      <c r="M110" s="5"/>
+      <c r="N110" s="16"/>
+      <c r="O110" s="2"/>
+    </row>
+    <row r="111" spans="3:15">
+      <c r="C111" s="5">
+        <v>110</v>
+      </c>
+      <c r="D111" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E111" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="F111" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G111" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H111" s="11"/>
+      <c r="I111" s="11"/>
+      <c r="J111" s="5"/>
+      <c r="K111" s="5"/>
+      <c r="L111" s="5"/>
+      <c r="M111" s="5"/>
+      <c r="N111" s="16"/>
+      <c r="O111" s="2"/>
+    </row>
+    <row r="112" spans="3:15">
+      <c r="C112" s="5">
+        <v>111</v>
+      </c>
+      <c r="D112" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E112" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G112" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H112" s="11" t="s">
+        <v>866</v>
+      </c>
+      <c r="I112" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="J112" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K112" s="5"/>
+      <c r="L112" s="5"/>
+      <c r="M112" s="5"/>
+      <c r="N112" s="16"/>
+      <c r="O112" s="2"/>
+    </row>
+    <row r="113" spans="3:15">
+      <c r="C113" s="5">
+        <v>112</v>
+      </c>
+      <c r="D113" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E113" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F113" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="G113" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H113" s="11" t="s">
+        <v>867</v>
+      </c>
+      <c r="I113" s="11"/>
+      <c r="J113" s="5"/>
+      <c r="K113" s="5"/>
+      <c r="L113" s="5"/>
+      <c r="M113" s="5"/>
+      <c r="N113" s="16"/>
+      <c r="O113" s="2"/>
+    </row>
+    <row r="114" spans="3:15">
+      <c r="C114" s="5">
+        <v>113</v>
+      </c>
+      <c r="D114" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E114" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G114" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H114" s="11" t="s">
+        <v>866</v>
+      </c>
+      <c r="I114" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="J114" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K114" s="5"/>
+      <c r="L114" s="5"/>
+      <c r="M114" s="5"/>
+      <c r="N114" s="16"/>
+      <c r="O114" s="2"/>
+    </row>
+    <row r="115" spans="3:15">
+      <c r="C115" s="5">
+        <v>114</v>
+      </c>
+      <c r="D115" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E115" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F115" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G115" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H115" s="11"/>
+      <c r="I115" s="11"/>
+      <c r="J115" s="5"/>
+      <c r="K115" s="5"/>
+      <c r="L115" s="5"/>
+      <c r="M115" s="5"/>
+      <c r="N115" s="16"/>
+      <c r="O115" s="2"/>
+    </row>
+    <row r="116" spans="3:15">
+      <c r="C116" s="5">
+        <v>115</v>
+      </c>
+      <c r="D116" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E116" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="G116" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H116" s="11" t="s">
+        <v>853</v>
+      </c>
+      <c r="I116" s="11"/>
+      <c r="J116" s="5"/>
+      <c r="K116" s="5"/>
+      <c r="L116" s="5"/>
+      <c r="M116" s="5"/>
+      <c r="N116" s="16"/>
+      <c r="O116" s="2"/>
+    </row>
+    <row r="117" spans="3:15">
+      <c r="C117" s="5">
+        <v>116</v>
+      </c>
+      <c r="D117" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E117" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="F117" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G117" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H117" s="11"/>
+      <c r="I117" s="11"/>
+      <c r="J117" s="5"/>
+      <c r="K117" s="5"/>
+      <c r="L117" s="5"/>
+      <c r="M117" s="5"/>
+      <c r="N117" s="16"/>
+      <c r="O117" s="2"/>
+    </row>
+    <row r="118" spans="3:15">
+      <c r="C118" s="5">
+        <v>117</v>
+      </c>
+      <c r="D118" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E118" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F118" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="G118" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H118" s="11" t="s">
+        <v>868</v>
+      </c>
+      <c r="I118" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="J118" s="11" t="s">
+        <v>869</v>
+      </c>
+      <c r="K118" s="5"/>
+      <c r="L118" s="5"/>
+      <c r="M118" s="5"/>
+      <c r="N118" s="16"/>
+      <c r="O118" s="2"/>
+    </row>
+    <row r="119" spans="3:15">
+      <c r="C119" s="5">
+        <v>118</v>
+      </c>
+      <c r="D119" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E119" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F119" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G119" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H119" s="11"/>
+      <c r="I119" s="11"/>
+      <c r="J119" s="5"/>
+      <c r="K119" s="5"/>
+      <c r="L119" s="5"/>
+      <c r="M119" s="5"/>
+      <c r="N119" s="16"/>
+      <c r="O119" s="2"/>
+    </row>
+    <row r="120" spans="3:15">
+      <c r="C120" s="5">
+        <v>119</v>
+      </c>
+      <c r="D120" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E120" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="F120" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G120" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H120" s="11"/>
+      <c r="I120" s="11"/>
+      <c r="J120" s="5"/>
+      <c r="K120" s="5"/>
+      <c r="L120" s="5"/>
+      <c r="M120" s="5"/>
+      <c r="N120" s="16"/>
+      <c r="O120" s="2"/>
+    </row>
+    <row r="121" spans="3:15">
+      <c r="C121" s="5">
+        <v>120</v>
+      </c>
+      <c r="D121" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E121" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="F121" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="G121" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H121" s="11" t="s">
+        <v>871</v>
+      </c>
+      <c r="I121" s="11"/>
+      <c r="J121" s="5"/>
+      <c r="K121" s="5"/>
+      <c r="L121" s="5"/>
+      <c r="M121" s="5"/>
+      <c r="N121" s="16"/>
+      <c r="O121" s="2"/>
+    </row>
+    <row r="122" spans="3:15">
+      <c r="C122" s="5">
+        <v>121</v>
+      </c>
+      <c r="D122" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E122" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="F122" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="G122" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H122" s="11"/>
+      <c r="I122" s="11"/>
+      <c r="J122" s="5"/>
+      <c r="K122" s="5"/>
+      <c r="L122" s="5"/>
+      <c r="M122" s="5"/>
+      <c r="N122" s="16"/>
+      <c r="O122" s="2"/>
+    </row>
+    <row r="123" spans="3:15">
+      <c r="C123" s="5">
+        <v>122</v>
+      </c>
+      <c r="D123" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E123" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G123" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H123" s="11"/>
+      <c r="I123" s="11"/>
+      <c r="J123" s="5"/>
+      <c r="K123" s="5"/>
+      <c r="L123" s="5"/>
+      <c r="M123" s="5"/>
+      <c r="N123" s="16"/>
+      <c r="O123" s="2"/>
+    </row>
+    <row r="124" spans="3:15" ht="15">
+      <c r="C124" s="5">
+        <v>123</v>
+      </c>
+      <c r="D124" s="6" t="s">
+        <v>784</v>
+      </c>
+      <c r="E124" s="11"/>
+      <c r="F124" s="5"/>
+      <c r="G124" s="5"/>
+      <c r="H124" s="11"/>
+      <c r="I124" s="11"/>
+      <c r="J124" s="5"/>
+      <c r="K124" s="5"/>
+      <c r="L124" s="5"/>
+      <c r="M124" s="5"/>
+      <c r="N124" s="16"/>
+      <c r="O124" s="2"/>
+    </row>
+    <row r="125" spans="3:15">
+      <c r="C125" s="5">
+        <v>124</v>
+      </c>
+      <c r="D125" s="18" t="s">
+        <v>786</v>
+      </c>
+      <c r="E125" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F125" s="11" t="s">
+        <v>821</v>
+      </c>
+      <c r="G125" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H125" s="11"/>
+      <c r="I125" s="5"/>
+      <c r="J125" s="5"/>
+      <c r="K125" s="5"/>
+      <c r="L125" s="5"/>
+      <c r="M125" s="5"/>
+      <c r="N125" s="21"/>
+      <c r="O125" s="22"/>
+    </row>
+    <row r="126" spans="3:15">
+      <c r="C126" s="5">
+        <v>125</v>
+      </c>
+      <c r="D126" s="18" t="s">
+        <v>786</v>
+      </c>
+      <c r="E126" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F126" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G126" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H126" s="11"/>
+      <c r="I126" s="5"/>
+      <c r="J126" s="5"/>
+      <c r="K126" s="5"/>
+      <c r="L126" s="5"/>
+      <c r="M126" s="5"/>
+      <c r="N126" s="21"/>
+      <c r="O126" s="22"/>
+    </row>
+    <row r="127" spans="3:15">
+      <c r="C127" s="5">
+        <v>126</v>
+      </c>
+      <c r="D127" s="18" t="s">
+        <v>822</v>
+      </c>
+      <c r="E127" s="11" t="s">
+        <v>823</v>
+      </c>
+      <c r="F127" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G127" s="11" t="s">
+        <v>824</v>
+      </c>
+      <c r="H127" s="11" t="s">
+        <v>825</v>
+      </c>
+      <c r="I127" s="5"/>
+      <c r="J127" s="5"/>
+      <c r="K127" s="5"/>
+      <c r="L127" s="5"/>
+      <c r="M127" s="5"/>
+      <c r="N127" s="21"/>
+      <c r="O127" s="22"/>
+    </row>
+    <row r="128" spans="3:15">
+      <c r="C128" s="5">
+        <v>127</v>
+      </c>
+      <c r="D128" s="18" t="s">
+        <v>822</v>
+      </c>
+      <c r="E128" s="11" t="s">
+        <v>823</v>
+      </c>
+      <c r="F128" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G128" s="11" t="s">
+        <v>824</v>
+      </c>
+      <c r="H128" s="11" t="s">
+        <v>826</v>
+      </c>
+      <c r="I128" s="5"/>
+      <c r="J128" s="5"/>
+      <c r="K128" s="5"/>
+      <c r="L128" s="5"/>
+      <c r="M128" s="5"/>
+      <c r="N128" s="21"/>
+      <c r="O128" s="22"/>
+    </row>
+    <row r="129" spans="3:15">
+      <c r="C129" s="5">
+        <v>128</v>
+      </c>
+      <c r="D129" s="18" t="s">
+        <v>822</v>
+      </c>
+      <c r="E129" s="11" t="s">
+        <v>823</v>
+      </c>
+      <c r="F129" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G129" s="11" t="s">
+        <v>824</v>
+      </c>
+      <c r="H129" s="11" t="s">
+        <v>827</v>
+      </c>
+      <c r="I129" s="5"/>
+      <c r="J129" s="5"/>
+      <c r="K129" s="5"/>
+      <c r="L129" s="5"/>
+      <c r="M129" s="5"/>
+      <c r="N129" s="21"/>
+      <c r="O129" s="22"/>
+    </row>
+    <row r="130" spans="3:15">
+      <c r="C130" s="5">
+        <v>129</v>
+      </c>
+      <c r="D130" s="18" t="s">
+        <v>822</v>
+      </c>
+      <c r="E130" s="11" t="s">
+        <v>823</v>
+      </c>
+      <c r="F130" s="11" t="s">
+        <v>828</v>
+      </c>
+      <c r="G130" s="11" t="s">
+        <v>829</v>
+      </c>
+      <c r="H130" s="11"/>
+      <c r="I130" s="5"/>
+      <c r="J130" s="5"/>
+      <c r="K130" s="5"/>
+      <c r="L130" s="5"/>
+      <c r="M130" s="5"/>
+      <c r="N130" s="21"/>
+      <c r="O130" s="22"/>
+    </row>
+    <row r="131" spans="3:15">
+      <c r="C131" s="5">
+        <v>130</v>
+      </c>
+      <c r="D131" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E131" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F131" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="G131" s="5" t="s">
+        <v>792</v>
+      </c>
+      <c r="H131" s="5"/>
+      <c r="I131" s="11"/>
+      <c r="J131" s="5"/>
+      <c r="K131" s="5"/>
+      <c r="L131" s="5"/>
+      <c r="M131" s="5"/>
+      <c r="N131" s="17"/>
+    </row>
+    <row r="132" spans="3:15">
+      <c r="C132" s="5">
+        <v>131</v>
+      </c>
+      <c r="D132" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E132" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F132" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G132" s="5" t="s">
+        <v>792</v>
+      </c>
+      <c r="H132" s="11"/>
+      <c r="I132" s="5"/>
+      <c r="J132" s="5"/>
+      <c r="K132" s="5"/>
+      <c r="L132" s="5"/>
+      <c r="M132" s="5"/>
+      <c r="N132" s="16"/>
+    </row>
+    <row r="133" spans="3:15">
+      <c r="C133" s="5">
+        <v>132</v>
+      </c>
+      <c r="D133" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E133" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F133" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G133" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H133" s="11" t="s">
+        <v>800</v>
+      </c>
+      <c r="I133" s="11"/>
+      <c r="J133" s="5"/>
+      <c r="K133" s="5"/>
+      <c r="L133" s="5"/>
+      <c r="M133" s="5"/>
+      <c r="N133" s="17"/>
+    </row>
+    <row r="134" spans="3:15">
+      <c r="C134" s="5">
+        <v>133</v>
+      </c>
+      <c r="D134" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E134" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F134" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="G134" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H134" s="5"/>
+      <c r="I134" s="5"/>
+      <c r="J134" s="5"/>
+      <c r="K134" s="5"/>
+      <c r="L134" s="5"/>
+      <c r="M134" s="5"/>
+      <c r="N134" s="16"/>
+    </row>
+    <row r="135" spans="3:15">
+      <c r="C135" s="5">
+        <v>137</v>
+      </c>
+      <c r="D135" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E135" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F135" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="G135" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H135" s="11" t="s">
+        <v>847</v>
+      </c>
+      <c r="I135" s="5"/>
+      <c r="J135" s="5"/>
+      <c r="K135" s="5"/>
+      <c r="L135" s="5"/>
+      <c r="M135" s="5"/>
+      <c r="N135" s="17"/>
+    </row>
+    <row r="136" spans="3:15">
+      <c r="C136" s="5">
+        <v>138</v>
+      </c>
+      <c r="D136" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E136" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F136" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="G136" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H136" s="5"/>
+      <c r="I136" s="5"/>
+      <c r="J136" s="5"/>
+      <c r="K136" s="5"/>
+      <c r="L136" s="5"/>
+      <c r="M136" s="5"/>
+      <c r="N136" s="17"/>
+    </row>
+    <row r="137" spans="3:15">
+      <c r="C137" s="5">
+        <v>139</v>
+      </c>
+      <c r="D137" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E137" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F137" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G137" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H137" s="11"/>
+      <c r="I137" s="5"/>
+      <c r="J137" s="5"/>
+      <c r="K137" s="5"/>
+      <c r="L137" s="5"/>
+      <c r="M137" s="5"/>
+      <c r="N137" s="16"/>
+    </row>
+    <row r="138" spans="3:15">
+      <c r="C138" s="5">
+        <v>140</v>
+      </c>
+      <c r="D138" s="8" t="s">
+        <v>819</v>
+      </c>
+      <c r="E138" s="11" t="s">
+        <v>794</v>
+      </c>
+      <c r="F138" s="5">
+        <v>2</v>
+      </c>
+      <c r="G138" s="5"/>
+      <c r="H138" s="11"/>
+      <c r="I138" s="5"/>
+      <c r="J138" s="5"/>
+      <c r="K138" s="5"/>
+      <c r="L138" s="5"/>
+      <c r="M138" s="5"/>
+      <c r="N138" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="N2:N67">
-    <cfRule type="cellIs" dxfId="1" priority="45" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="N2:N138">
+    <cfRule type="cellIs" dxfId="1" priority="51" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="46" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="52" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E39 F2:F67">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E62 F2:F138">
       <formula1>OFFSET(INDIRECT($E2),0,0,COUNTA(INDIRECT(D2&amp;"Col")),1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D58:D67 D3:D4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D105:D107 D79:D99 D3:D4 D6:D28 D132:D138">
       <formula1>"C,F,T,;"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E38 E40:E67">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E61 E63:E138">
       <formula1>Forms</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G67">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G138">
       <formula1>INDIRECT(SUBSTITUTE(E2&amp;F2," ",""))</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="H14" r:id="rId1"/>
-    <hyperlink ref="H15" r:id="rId2"/>
+    <hyperlink ref="H38" r:id="rId1"/>
+    <hyperlink ref="H39" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -28579,39 +30522,39 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>839</v>
+        <v>831</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>840</v>
+        <v>832</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>841</v>
+        <v>833</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>842</v>
+        <v>834</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>843</v>
+        <v>835</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>844</v>
+        <v>836</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>845</v>
+        <v>837</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>846</v>
+        <v>838</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>847</v>
+        <v>839</v>
       </c>
       <c r="B5" s="10">
         <v>41116</v>
@@ -28619,7 +30562,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>848</v>
+        <v>840</v>
       </c>
       <c r="B6" s="10">
         <v>41116</v>
@@ -28630,18 +30573,18 @@
         <v>765</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>849</v>
+        <v>841</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
-        <v>850</v>
+        <v>842</v>
       </c>
       <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
-        <v>851</v>
+        <v>843</v>
       </c>
       <c r="B9" s="12"/>
     </row>

</xml_diff>